<commit_message>
organized files and folders
</commit_message>
<xml_diff>
--- a/Template/תבנית זמינות.xlsx
+++ b/Template/תבנית זמינות.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orbac\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orbac\Desktop\Shift-Schedule\Shift-Schedule\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69BF779-5E19-434C-B716-3525C69C49C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B71B9B-DAA4-4E4F-8EF5-782E2D323C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2115" yWindow="2115" windowWidth="22155" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>א</t>
   </si>
@@ -250,34 +250,7 @@
     <t xml:space="preserve"> אותיות:</t>
   </si>
   <si>
-    <t>זיו</t>
-  </si>
-  <si>
-    <t>אור</t>
-  </si>
-  <si>
-    <t>רוני</t>
-  </si>
-  <si>
-    <t xml:space="preserve">אמור </t>
-  </si>
-  <si>
-    <t>אוראל</t>
-  </si>
-  <si>
-    <t>יניב</t>
-  </si>
-  <si>
-    <t>עמית</t>
-  </si>
-  <si>
-    <t>a.b</t>
-  </si>
-  <si>
-    <t>b.c</t>
-  </si>
-  <si>
-    <t>a.c</t>
+    <t>כמות לילות:</t>
   </si>
 </sst>
 </file>
@@ -626,7 +599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -700,14 +673,38 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -728,11 +725,31 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$I$2" max="6" page="10" val="4"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$I$2" max="6" page="10" val="6"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$K$4" max="30000" page="10" val="2"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$K$5" max="30000" page="10" val="2"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$K$6" max="30000" page="10" val="2"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$K$7" max="30000" page="10" val="2"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$K$8" max="30000" page="10" val="2"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$I$3" max="6" page="10" val="5"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$I$3" max="6" page="10" val="6"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -748,11 +765,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$I$7" max="6" page="10" val="4"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$I$7" max="6" page="10" val="6"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$I$8" max="6" page="10" val="5"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$I$8" max="6" page="10" val="6"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$K$2" max="30000" page="10" val="2"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$K$3" max="30000" page="10" val="2"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -762,15 +787,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>91440</xdr:colOff>
+          <xdr:colOff>95250</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -812,15 +837,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>91440</xdr:colOff>
+          <xdr:colOff>95250</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -862,15 +887,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>91440</xdr:colOff>
+          <xdr:colOff>95250</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -914,13 +939,13 @@
           <xdr:col>8</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>60960</xdr:rowOff>
+          <xdr:rowOff>57150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>251460</xdr:colOff>
+          <xdr:colOff>247650</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>213360</xdr:rowOff>
+          <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -968,7 +993,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>251460</xdr:colOff>
+          <xdr:colOff>247650</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
@@ -1014,13 +1039,13 @@
           <xdr:col>8</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>60960</xdr:rowOff>
+          <xdr:rowOff>57150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>251460</xdr:colOff>
+          <xdr:colOff>247650</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>213360</xdr:rowOff>
+          <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1062,15 +1087,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>60960</xdr:colOff>
+          <xdr:colOff>57150</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>53340</xdr:rowOff>
+          <xdr:rowOff>57150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>251460</xdr:colOff>
+          <xdr:colOff>247650</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1081,6 +1106,356 @@
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>323850</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>514350</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1033" name="Spinner 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1033"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>314740</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>71230</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>505240</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>223630</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1034" name="Spinner 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1034"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13C52A33-D12C-8D34-54B3-55AF9EAC8257}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>312254</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>57978</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>502754</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>213691</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1035" name="Spinner 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1035"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A84E56AE-8E43-0FD2-E55D-96D408D5787A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>320537</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>41412</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>511037</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>197125</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1036" name="Spinner 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1036"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A17D6D91-7EF7-3065-1243-49D89278B7C2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>320537</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>49696</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>511037</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>205409</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1037" name="Spinner 13" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1037"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CFDBEC2-7A03-FE46-0A72-C08DD3B52009}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>320537</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>49695</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>511037</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>205408</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1038" name="Spinner 14" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1038"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9C3BF1D-2053-CC1A-EA81-34D4C3AA6D3D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>312254</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>49695</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>502754</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>205408</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1039" name="Spinner 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1039"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0ABC47E-8381-8188-5B1D-688F7AF22452}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1377,27 +1752,27 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1"/>
-    <col min="10" max="10" width="3.109375" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.140625" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1"/>
     <col min="12" max="12" width="3" customWidth="1"/>
-    <col min="13" max="13" width="24.77734375" customWidth="1"/>
-    <col min="14" max="14" width="2.44140625" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" customWidth="1"/>
+    <col min="14" max="14" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="16" t="s">
         <v>0</v>
@@ -1424,206 +1799,138 @@
         <v>10</v>
       </c>
       <c r="J1" s="9"/>
+      <c r="K1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>36</v>
-      </c>
+    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
       <c r="I2" s="19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J2" s="5"/>
+      <c r="K2" s="38">
+        <v>2</v>
+      </c>
+      <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:14" ht="21.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
+    <row r="3" spans="1:14" ht="21.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
       <c r="I3" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J3" s="5"/>
+      <c r="K3" s="39">
+        <v>2</v>
+      </c>
+      <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:14" ht="20.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>36</v>
-      </c>
+    <row r="4" spans="1:14" ht="20.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="23">
         <v>6</v>
       </c>
       <c r="J4" s="5"/>
+      <c r="K4" s="40">
+        <v>2</v>
+      </c>
+      <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
-        <v>32</v>
-      </c>
+    <row r="5" spans="1:14" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="25">
         <v>6</v>
       </c>
       <c r="J5" s="5"/>
+      <c r="K5" s="41">
+        <v>2</v>
+      </c>
+      <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>16</v>
-      </c>
+    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
       <c r="I6" s="27">
         <v>6</v>
       </c>
       <c r="J6" s="5"/>
+      <c r="K6" s="42">
+        <v>2</v>
+      </c>
+      <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
+    <row r="7" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
       <c r="I7" s="29">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J7" s="5"/>
+      <c r="K7" s="43">
+        <v>2</v>
+      </c>
+      <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:14" ht="18.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="30" t="s">
-        <v>35</v>
-      </c>
+    <row r="8" spans="1:14" ht="18.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="30"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>16</v>
-      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="14" t="s">
-        <v>15</v>
-      </c>
+      <c r="H8" s="14"/>
       <c r="I8" s="31">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J8" s="5"/>
+      <c r="K8" s="44">
+        <v>2</v>
+      </c>
+      <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
         <v>23</v>
       </c>
@@ -1648,12 +1955,16 @@
       <c r="H9" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="35">
+      <c r="I9" s="37">
         <v>6</v>
       </c>
       <c r="J9" s="5"/>
+      <c r="K9" s="45">
+        <v>6</v>
+      </c>
+      <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1664,8 +1975,10 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:14" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>27</v>
       </c>
@@ -1692,8 +2005,10 @@
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1709,19 +2024,19 @@
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
       <c r="J13" s="5"/>
       <c r="K13" s="6" t="s">
         <v>7</v>
@@ -1732,16 +2047,16 @@
       </c>
       <c r="N13" s="10"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="36" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
       <c r="J14" s="5"/>
       <c r="K14" s="7" t="s">
         <v>17</v>
@@ -1752,16 +2067,16 @@
       </c>
       <c r="N14" s="5"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="36" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
       <c r="J15" s="5"/>
       <c r="K15" s="8" t="s">
         <v>18</v>
@@ -1772,16 +2087,16 @@
       </c>
       <c r="N15" s="5"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="36" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
       <c r="K16" s="8" t="s">
         <v>19</v>
       </c>
@@ -1791,16 +2106,16 @@
       </c>
       <c r="N16" s="5"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="36" t="s">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
       <c r="K17" s="7" t="s">
         <v>20</v>
       </c>
@@ -1810,7 +2125,7 @@
       </c>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K18" s="8" t="s">
         <v>9</v>
       </c>
@@ -1818,13 +2133,13 @@
       <c r="M18" s="12"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K20" s="8" t="s">
         <v>25</v>
       </c>
@@ -1834,7 +2149,7 @@
       </c>
       <c r="N20" s="5"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K21" s="8" t="s">
         <v>26</v>
       </c>
@@ -1844,7 +2159,7 @@
       </c>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L22" s="5"/>
       <c r="N22" s="5"/>
     </row>
@@ -1865,15 +2180,15 @@
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>91440</xdr:colOff>
+                    <xdr:colOff>95250</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>8</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>175260</xdr:rowOff>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1887,15 +2202,15 @@
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>91440</xdr:colOff>
+                    <xdr:colOff>95250</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>8</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>175260</xdr:rowOff>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1909,15 +2224,15 @@
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>91440</xdr:colOff>
+                    <xdr:colOff>95250</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>8</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>175260</xdr:rowOff>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1933,13 +2248,13 @@
                     <xdr:col>8</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>60960</xdr:rowOff>
+                    <xdr:rowOff>57150</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>251460</xdr:colOff>
+                    <xdr:colOff>247650</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>213360</xdr:rowOff>
+                    <xdr:rowOff>209550</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1959,7 +2274,7 @@
                   </from>
                   <to>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>251460</xdr:colOff>
+                    <xdr:colOff>247650</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>190500</xdr:rowOff>
                   </to>
@@ -1977,13 +2292,13 @@
                     <xdr:col>8</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>60960</xdr:rowOff>
+                    <xdr:rowOff>57150</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>251460</xdr:colOff>
+                    <xdr:colOff>247650</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>213360</xdr:rowOff>
+                    <xdr:rowOff>209550</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1997,15 +2312,169 @@
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>60960</xdr:colOff>
+                    <xdr:colOff>57150</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>53340</xdr:rowOff>
+                    <xdr:rowOff>57150</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>251460</xdr:colOff>
+                    <xdr:colOff>247650</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>205740</xdr:rowOff>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1033" r:id="rId10" name="Spinner 9">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>323850</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>514350</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1034" r:id="rId11" name="Spinner 10">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>314325</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>504825</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>219075</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1035" r:id="rId12" name="Spinner 11">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>314325</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>57150</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>504825</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1036" r:id="rId13" name="Spinner 12">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>323850</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>514350</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1037" r:id="rId14" name="Spinner 13">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>323850</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>514350</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1038" r:id="rId15" name="Spinner 14">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>323850</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>514350</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1039" r:id="rId16" name="Spinner 15">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>314325</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>504825</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>

<commit_message>
added eightx2 shifts check
</commit_message>
<xml_diff>
--- a/Template/תבנית זמינות.xlsx
+++ b/Template/תבנית זמינות.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orbac\Desktop\Shift-Schedule\Shift-Schedule\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B71B9B-DAA4-4E4F-8EF5-782E2D323C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7F6CE2-8BD4-46CD-9F42-977BF31050ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="2115" windowWidth="22155" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>א</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>כמות לילות:</t>
+  </si>
+  <si>
+    <t>העדפה ללילות רצופים Y/N:</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -676,35 +682,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1187,15 +1193,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>314740</xdr:colOff>
+          <xdr:colOff>314325</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>71230</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>505240</xdr:colOff>
+          <xdr:colOff>504825</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>223630</xdr:rowOff>
+          <xdr:rowOff>219075</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1205,7 +1211,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13C52A33-D12C-8D34-54B3-55AF9EAC8257}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1237,15 +1243,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>312254</xdr:colOff>
+          <xdr:colOff>314325</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>57978</xdr:rowOff>
+          <xdr:rowOff>57150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>502754</xdr:colOff>
+          <xdr:colOff>504825</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>213691</xdr:rowOff>
+          <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1255,7 +1261,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A84E56AE-8E43-0FD2-E55D-96D408D5787A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1287,15 +1293,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>320537</xdr:colOff>
+          <xdr:colOff>323850</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>41412</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>511037</xdr:colOff>
+          <xdr:colOff>514350</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>197125</xdr:rowOff>
+          <xdr:rowOff>200025</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1305,7 +1311,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A17D6D91-7EF7-3065-1243-49D89278B7C2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1337,15 +1343,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>320537</xdr:colOff>
+          <xdr:colOff>323850</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>49696</xdr:rowOff>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>511037</xdr:colOff>
+          <xdr:colOff>514350</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>205409</xdr:rowOff>
+          <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1355,7 +1361,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CFDBEC2-7A03-FE46-0A72-C08DD3B52009}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1387,15 +1393,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>320537</xdr:colOff>
+          <xdr:colOff>323850</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>49695</xdr:rowOff>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>511037</xdr:colOff>
+          <xdr:colOff>514350</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>205408</xdr:rowOff>
+          <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1405,7 +1411,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9C3BF1D-2053-CC1A-EA81-34D4C3AA6D3D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1437,15 +1443,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>312254</xdr:colOff>
+          <xdr:colOff>314325</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>49695</xdr:rowOff>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>502754</xdr:colOff>
+          <xdr:colOff>504825</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>205408</xdr:rowOff>
+          <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1455,7 +1461,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0ABC47E-8381-8188-5B1D-688F7AF22452}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1751,8 +1757,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,6 +1809,9 @@
         <v>29</v>
       </c>
       <c r="L1" s="9"/>
+      <c r="M1" s="17" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
@@ -1817,10 +1826,13 @@
         <v>6</v>
       </c>
       <c r="J2" s="5"/>
-      <c r="K2" s="38">
+      <c r="K2" s="37">
         <v>2</v>
       </c>
       <c r="L2" s="5"/>
+      <c r="M2" s="37" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:14" ht="21.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
@@ -1835,10 +1847,13 @@
         <v>6</v>
       </c>
       <c r="J3" s="5"/>
-      <c r="K3" s="39">
+      <c r="K3" s="38">
         <v>2</v>
       </c>
       <c r="L3" s="5"/>
+      <c r="M3" s="38" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="20.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
@@ -1853,10 +1868,13 @@
         <v>6</v>
       </c>
       <c r="J4" s="5"/>
-      <c r="K4" s="40">
+      <c r="K4" s="39">
         <v>2</v>
       </c>
       <c r="L4" s="5"/>
+      <c r="M4" s="39" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:14" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
@@ -1871,10 +1889,13 @@
         <v>6</v>
       </c>
       <c r="J5" s="5"/>
-      <c r="K5" s="41">
+      <c r="K5" s="40">
         <v>2</v>
       </c>
       <c r="L5" s="5"/>
+      <c r="M5" s="40" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26"/>
@@ -1889,10 +1910,13 @@
         <v>6</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="K6" s="42">
+      <c r="K6" s="41">
         <v>2</v>
       </c>
       <c r="L6" s="5"/>
+      <c r="M6" s="41" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
@@ -1907,10 +1931,13 @@
         <v>6</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="43">
+      <c r="K7" s="42">
         <v>2</v>
       </c>
       <c r="L7" s="5"/>
+      <c r="M7" s="42" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="18.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30"/>
@@ -1925,10 +1952,13 @@
         <v>6</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="44">
+      <c r="K8" s="43">
         <v>2</v>
       </c>
       <c r="L8" s="5"/>
+      <c r="M8" s="43" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
@@ -1955,14 +1985,17 @@
       <c r="H9" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="37">
+      <c r="I9" s="36">
         <v>6</v>
       </c>
       <c r="J9" s="5"/>
-      <c r="K9" s="45">
+      <c r="K9" s="44">
         <v>6</v>
       </c>
       <c r="L9" s="5"/>
+      <c r="M9" s="44" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
@@ -2028,15 +2061,15 @@
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
       <c r="J13" s="5"/>
       <c r="K13" s="6" t="s">
         <v>7</v>

</xml_diff>